<commit_message>
Initial checkin for ACC pilot example
</commit_message>
<xml_diff>
--- a/specification/src/docs/SDC_HeD_Mapping.xlsx
+++ b/specification/src/docs/SDC_HeD_Mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
   <si>
     <t>Section_Element</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>List_Item</t>
+  </si>
+  <si>
+    <t>DocumentationItem</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1150,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1187,7 @@
         <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Mapping of SDC forms, specifically Question_Element's subtypes. Also reviewed mapping of the overall SDC forms structure but mapping has not started yet.
</commit_message>
<xml_diff>
--- a/specification/src/docs/SDC_HeD_Mapping.xlsx
+++ b/specification/src/docs/SDC_HeD_Mapping.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Section_Element" sheetId="1" r:id="rId1"/>
-    <sheet name="Question_Element" sheetId="2" r:id="rId2"/>
-    <sheet name="List_Field" sheetId="5" r:id="rId3"/>
-    <sheet name="Text_Field" sheetId="3" r:id="rId4"/>
+    <sheet name="form_package" sheetId="6" r:id="rId1"/>
+    <sheet name="Section_Element" sheetId="1" r:id="rId2"/>
+    <sheet name="Question_Element" sheetId="2" r:id="rId3"/>
+    <sheet name="List_Field" sheetId="5" r:id="rId4"/>
+    <sheet name="Text_Field" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="141">
   <si>
     <t>Section_Element</t>
   </si>
@@ -287,13 +288,178 @@
   </si>
   <si>
     <t>DocumentationItem</t>
+  </si>
+  <si>
+    <t>strictSelection</t>
+  </si>
+  <si>
+    <t>strictSelection = false is the same as fill_in = true</t>
+  </si>
+  <si>
+    <t>EnumerationConstraint/item</t>
+  </si>
+  <si>
+    <t>This is a type that is defined inline in HeD</t>
+  </si>
+  <si>
+    <t>item_prompt_xhtmldefault_element</t>
+  </si>
+  <si>
+    <t>anyType</t>
+  </si>
+  <si>
+    <t>displayText</t>
+  </si>
+  <si>
+    <t>media_element</t>
+  </si>
+  <si>
+    <t>guard</t>
+  </si>
+  <si>
+    <t>Inline type</t>
+  </si>
+  <si>
+    <t>value_meaning_terminology_code_</t>
+  </si>
+  <si>
+    <t>list_item_order</t>
+  </si>
+  <si>
+    <t>list_item_identifier</t>
+  </si>
+  <si>
+    <t>Not clear what purpose it serves</t>
+  </si>
+  <si>
+    <t>codes</t>
+  </si>
+  <si>
+    <t>Assume guard constrains if this item is shown based on the selection of another item</t>
+  </si>
+  <si>
+    <t>Is it needed?</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>HeD allows more than String values</t>
+  </si>
+  <si>
+    <t>item_number</t>
+  </si>
+  <si>
+    <t>item_prompt</t>
+  </si>
+  <si>
+    <t>Additional_Text</t>
+  </si>
+  <si>
+    <t>value_meaning</t>
+  </si>
+  <si>
+    <t>What does it mean to fill in an item value?</t>
+  </si>
+  <si>
+    <t>guarded</t>
+  </si>
+  <si>
+    <t>multiselect</t>
+  </si>
+  <si>
+    <t>Not sure of the use of multiselect with a text field.</t>
+  </si>
+  <si>
+    <t>ResponseCardinality</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>default_value_read_only</t>
+  </si>
+  <si>
+    <t>maximum_character_quantity</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>unit_of_measure</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>How does this interact with the ordering and guarding?</t>
+  </si>
+  <si>
+    <t>How is this different than default_value</t>
+  </si>
+  <si>
+    <t>How is this different than allowing the entire element to be editable?</t>
+  </si>
+  <si>
+    <t>Written as expression constraint</t>
+  </si>
+  <si>
+    <t>If entry is for quantity, then responseDataType is physical quantity</t>
+  </si>
+  <si>
+    <t>How is this different than datatype?</t>
+  </si>
+  <si>
+    <t>This is like a mask. Such expressions are not currently supported.</t>
+  </si>
+  <si>
+    <t>MaskConstraint</t>
+  </si>
+  <si>
+    <t>form_package element</t>
+  </si>
+  <si>
+    <t>inline type</t>
+  </si>
+  <si>
+    <t>KnowledgeDocument</t>
+  </si>
+  <si>
+    <t>mapping_package</t>
+  </si>
+  <si>
+    <t>administrative_package</t>
+  </si>
+  <si>
+    <t>stylesheet</t>
+  </si>
+  <si>
+    <t>form_design</t>
+  </si>
+  <si>
+    <t>supplemental_data</t>
+  </si>
+  <si>
+    <t>form_package_identifier</t>
+  </si>
+  <si>
+    <t>form_design_identifier</t>
+  </si>
+  <si>
+    <t>Do not understand how this works</t>
+  </si>
+  <si>
+    <t>What is this for?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,8 +489,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +516,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -370,6 +549,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +837,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,12 +1230,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,17 +1458,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -1183,13 +1496,15 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1239,7 +1554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1248,6 +1563,12 @@
       </c>
       <c r="C7" t="s">
         <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,22 +1582,227 @@
         <v>84</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -1312,7 +1838,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1322,11 +1848,9 @@
       <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>78</v>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,6 +1865,132 @@
       </c>
       <c r="D5" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refinements to HeD schema to better align with SDC. Added example of SDC form translated to HeD.
</commit_message>
<xml_diff>
--- a/specification/src/docs/SDC_HeD_Mapping.xlsx
+++ b/specification/src/docs/SDC_HeD_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="form_package" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Question_Element" sheetId="2" r:id="rId3"/>
     <sheet name="List_Field" sheetId="5" r:id="rId4"/>
     <sheet name="Text_Field" sheetId="3" r:id="rId5"/>
+    <sheet name="DE Read only" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="161">
   <si>
     <t>Section_Element</t>
   </si>
@@ -156,9 +157,6 @@
     <t>Resolved</t>
   </si>
   <si>
-    <t>The Media_Element type has no usable attributes currently.</t>
-  </si>
-  <si>
     <t>supportingResources</t>
   </si>
   <si>
@@ -241,9 +239,6 @@
   </si>
   <si>
     <t>With range constraint type called EnumerationConstraint</t>
-  </si>
-  <si>
-    <t>Use is unclear</t>
   </si>
   <si>
     <t>DocumentationConcept</t>
@@ -335,12 +330,6 @@
     <t>codes</t>
   </si>
   <si>
-    <t>Assume guard constrains if this item is shown based on the selection of another item</t>
-  </si>
-  <si>
-    <t>Is it needed?</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -359,21 +348,12 @@
     <t>value_meaning</t>
   </si>
   <si>
-    <t>What does it mean to fill in an item value?</t>
-  </si>
-  <si>
     <t>guarded</t>
   </si>
   <si>
     <t>multiselect</t>
   </si>
   <si>
-    <t>Not sure of the use of multiselect with a text field.</t>
-  </si>
-  <si>
-    <t>ResponseCardinality</t>
-  </si>
-  <si>
     <t>default_value</t>
   </si>
   <si>
@@ -395,15 +375,9 @@
     <t>format</t>
   </si>
   <si>
-    <t>How does this interact with the ordering and guarding?</t>
-  </si>
-  <si>
     <t>How is this different than default_value</t>
   </si>
   <si>
-    <t>How is this different than allowing the entire element to be editable?</t>
-  </si>
-  <si>
     <t>Written as expression constraint</t>
   </si>
   <si>
@@ -413,12 +387,6 @@
     <t>How is this different than datatype?</t>
   </si>
   <si>
-    <t>This is like a mask. Such expressions are not currently supported.</t>
-  </si>
-  <si>
-    <t>MaskConstraint</t>
-  </si>
-  <si>
     <t>form_package element</t>
   </si>
   <si>
@@ -453,13 +421,107 @@
   </si>
   <si>
     <t>What is this for?</t>
+  </si>
+  <si>
+    <t># of DEs: 4</t>
+  </si>
+  <si>
+    <t>do you breats cancer?</t>
+  </si>
+  <si>
+    <t>do you have lung cancer?</t>
+  </si>
+  <si>
+    <t>do you have prostate cancer?</t>
+  </si>
+  <si>
+    <t>do you have ovarian cancer?</t>
+  </si>
+  <si>
+    <t>Cancer indicator</t>
+  </si>
+  <si>
+    <t>Body Location</t>
+  </si>
+  <si>
+    <t># of DE: 2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Breast</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>Prostate</t>
+  </si>
+  <si>
+    <t>Ovarian</t>
+  </si>
+  <si>
+    <t>To construct a table view</t>
+  </si>
+  <si>
+    <t>Added element called textAfterResponse in DocumentationItem</t>
+  </si>
+  <si>
+    <t>Added new element called scopedIdentifier to ItemDefinition</t>
+  </si>
+  <si>
+    <t>Added new element called number to ActionBase (parent of CollectInformationAction)</t>
+  </si>
+  <si>
+    <t>The Media_Element type has no usable attributes currently. Discussion with Mark indicates the requirements are not clear.</t>
+  </si>
+  <si>
+    <t>Added identifier to EnumerationItem</t>
+  </si>
+  <si>
+    <t>Added number to EnumerationItem</t>
+  </si>
+  <si>
+    <t>Added new type called MaskConstraint. This is like a mask. Such expressions are not currently supported.</t>
+  </si>
+  <si>
+    <t>Resolved.</t>
+  </si>
+  <si>
+    <t>This is an error in the sDC schema</t>
+  </si>
+  <si>
+    <t>In HeD, the guards are placed on the item being guarded. This is specified as applicable scenarios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Mark: "An explicit reference to the next element to be shown in the form design" Its an optional element that is used when there is a "Guarded_Element" in-line with the question/list item.  Once the flow through the XML hits that element, it may not be clear which item to move to next.  Maybe there is another way to do that…
+</t>
+  </si>
+  <si>
+    <t>In HeD, items are already ordered. Guards are placed on the item being guarded. If the item is applicable, it shows up where it is in the order. If not, the next applicable item is shown. Hence, no need for an explicit next_relevant_element.</t>
+  </si>
+  <si>
+    <t>Per Mark, this is an error in the SDC schema.</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Added new element called additionalInstruction</t>
+  </si>
+  <si>
+    <t>Create enumeration item with fillIn = true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,8 +558,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,8 +590,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -531,11 +611,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -557,6 +652,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -873,70 +987,72 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
-        <v>131</v>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -947,7 +1063,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -966,12 +1082,12 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -985,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1007,19 +1123,19 @@
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,10 +1160,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1104,7 +1220,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,7 +1234,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1150,7 +1266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1161,10 +1277,10 @@
         <v>31</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,7 +1351,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1263,9 +1379,7 @@
       <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="7"/>
@@ -1281,21 +1395,21 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1303,14 +1417,16 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" t="s">
-        <v>71</v>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1319,21 +1435,24 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1346,71 +1465,74 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>68</v>
-      </c>
-      <c r="E12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1418,14 +1540,16 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" t="s">
-        <v>71</v>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -1440,7 +1564,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1462,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1595,7 @@
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1482,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1497,46 +1621,46 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1556,7 +1680,7 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1565,52 +1689,52 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -1618,29 +1742,33 @@
       <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="D15" s="19"/>
       <c r="E15" s="7" t="s">
-        <v>101</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1649,28 +1777,28 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1678,14 +1806,16 @@
       <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1694,15 +1824,15 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1710,14 +1840,17 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>106</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1726,10 +1859,10 @@
         <v>20</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1737,28 +1870,31 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1766,14 +1902,16 @@
       <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1781,10 +1919,13 @@
       <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" t="s">
-        <v>99</v>
-      </c>
+      <c r="D25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1794,21 +1935,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1816,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1826,50 +1968,49 @@
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
       <c r="D5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1878,15 +2019,16 @@
         <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1895,15 +2037,15 @@
         <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1912,27 +2054,30 @@
         <v>25</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1940,13 +2085,13 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1955,15 +2100,15 @@
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1972,13 +2117,13 @@
         <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1988,12 +2133,128 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" t="s">
-        <v>121</v>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ordering to HeD ActionBase to support SDC order in form definitions.
</commit_message>
<xml_diff>
--- a/specification/src/docs/SDC_HeD_Mapping.xlsx
+++ b/specification/src/docs/SDC_HeD_Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aziz\Dev\repos\cqframework\healthedecisions\specification\src\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\SS\KAS\specification\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="607" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="form_package" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Text_Field" sheetId="3" r:id="rId5"/>
     <sheet name="DE Read only" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="165">
   <si>
     <t>Section_Element</t>
   </si>
@@ -515,13 +518,25 @@
   </si>
   <si>
     <t>Create enumeration item with fillIn = true</t>
+  </si>
+  <si>
+    <t>e.g. M</t>
+  </si>
+  <si>
+    <t>HTML Display text associated with the list item</t>
+  </si>
+  <si>
+    <t>Not able to find the semantics for this nor an example of usage. We will exclude from this round of alignment.</t>
+  </si>
+  <si>
+    <t>Added order attribute to ActionBase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,13 +562,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -630,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -651,32 +659,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1082,7 +1116,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,9 +1238,11 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="7" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,9 +1297,11 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1351,7 +1389,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,9 +1595,11 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="7" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1635,8 @@
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1729,8 +1770,12 @@
       <c r="C13" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1750,7 +1795,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -1760,11 +1805,15 @@
       <c r="C15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E15" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1781,7 +1830,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1791,9 +1840,11 @@
       <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E17" s="7" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1829,6 +1880,9 @@
       <c r="E19" s="11" t="s">
         <v>100</v>
       </c>
+      <c r="F19" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1929,7 +1983,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1937,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +2072,7 @@
       <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -2054,7 +2108,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>144</v>
       </c>
       <c r="G8" t="s">
@@ -2102,7 +2156,7 @@
       <c r="D11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2133,11 +2187,13 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2162,96 +2218,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to add VisualStyleBehavior and ReadOnlyBehavior to the schema.
</commit_message>
<xml_diff>
--- a/specification/src/docs/SDC_HeD_Mapping.xlsx
+++ b/specification/src/docs/SDC_HeD_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="607" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="607" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="form_package" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1115,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1991,7 +1991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>